<commit_message>
computed for n=1200, 6sentences transformers models, 8ML models, results bad.
</commit_message>
<xml_diff>
--- a/predictive_data_Meta ACA_without_searching.xlsx
+++ b/predictive_data_Meta ACA_without_searching.xlsx
@@ -460,10 +460,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.8129032258064516</v>
+        <v>0.7</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7563298490127759</v>
+        <v>0.5838986883763003</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -471,7 +471,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -479,10 +479,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.8193548387096774</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7728222996515679</v>
+        <v>0.5764360018091361</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1200</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>